<commit_message>
Excel, luu tru du lieu cho he thong
</commit_message>
<xml_diff>
--- a/QuanLyChiTieu/Data/Account.xlsx
+++ b/QuanLyChiTieu/Data/Account.xlsx
@@ -707,8 +707,8 @@
     <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
   <tableStyles count="2" defaultTableStyle="TableStylePreset3_Accent1 1" defaultPivotStyle="PivotStylePreset2_Accent1 1">
-    <tableStyle name="TableStylePreset3_Accent1 1" pivot="0" count="0" xr9:uid="{1F30E028-89DD-4B64-90F1-C24F11A1B807}"/>
-    <tableStyle name="PivotStylePreset2_Accent1 1" table="0" count="0" xr9:uid="{378C6032-4626-4A36-9EA1-FC6239F0A6CA}"/>
+    <tableStyle name="TableStylePreset3_Accent1 1" pivot="0" count="0" xr9:uid="{9272F313-5115-4C4A-A997-D2C86209E92E}"/>
+    <tableStyle name="PivotStylePreset2_Accent1 1" table="0" count="0" xr9:uid="{B41F7AE8-7AD8-4300-A324-05A0A8618CE3}"/>
   </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1006,7 +1006,7 @@
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="A2:B3"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="1"/>

</xml_diff>

<commit_message>
Commit changes to various files
</commit_message>
<xml_diff>
--- a/QuanLyChiTieu/Data/Account.xlsx
+++ b/QuanLyChiTieu/Data/Account.xlsx
@@ -43,6 +43,9 @@
   </x:si>
   <x:si>
     <x:t>kikaho</x:t>
+  </x:si>
+  <x:si>
+    <x:t>HoaiBao</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -1054,6 +1057,14 @@
         <x:v>3</x:v>
       </x:c>
     </x:row>
+    <x:row r="4" spans="1:2">
+      <x:c r="A4" s="0" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="B4" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>

</xml_diff>

<commit_message>
sua truc tiep tren bang hien thi
</commit_message>
<xml_diff>
--- a/QuanLyChiTieu/Data/Account.xlsx
+++ b/QuanLyChiTieu/Data/Account.xlsx
@@ -36,13 +36,13 @@
     <x:t>Mật khẩu</x:t>
   </x:si>
   <x:si>
-    <x:t>nha123vo</x:t>
+    <x:t>kikaho</x:t>
   </x:si>
   <x:si>
     <x:t>123456aA@</x:t>
   </x:si>
   <x:si>
-    <x:t>kikaho</x:t>
+    <x:t>vtn26xn</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -724,8 +724,8 @@
     <x:cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </x:cellStyles>
   <x:tableStyles count="2" defaultTableStyle="TableStylePreset3_Accent1 1" defaultPivotStyle="PivotStylePreset2_Accent1 1">
-    <x:tableStyle name="TableStylePreset3_Accent1 1" pivot="0" count="0" xr9:uid="{9272F313-5115-4C4A-A997-D2C86209E92E}"/>
-    <x:tableStyle name="PivotStylePreset2_Accent1 1" table="0" count="0" xr9:uid="{B41F7AE8-7AD8-4300-A324-05A0A8618CE3}"/>
+    <x:tableStyle name="TableStylePreset3_Accent1 1" pivot="0" count="0" xr9:uid="{4E991D03-7791-4C01-8C61-C97CF5DB67EB}"/>
+    <x:tableStyle name="PivotStylePreset2_Accent1 1" table="0" count="0" xr9:uid="{0D5EF9CF-D092-487A-AE9E-C797031E8A91}"/>
   </x:tableStyles>
   <x:extLst>
     <x:ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1025,7 +1025,7 @@
   <x:dimension ref="A1:B1"/>
   <x:sheetViews>
     <x:sheetView tabSelected="1" workbookViewId="0">
-      <x:selection activeCell="G15" sqref="G15"/>
+      <x:selection activeCell="B3" sqref="B3 A2:B3"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultColWidth="8.996339" defaultRowHeight="14.4"/>

</xml_diff>

<commit_message>
chỉnh sửa giao dịch
</commit_message>
<xml_diff>
--- a/QuanLyChiTieu/Data/Account.xlsx
+++ b/QuanLyChiTieu/Data/Account.xlsx
@@ -40,6 +40,9 @@
   </x:si>
   <x:si>
     <x:t>123456aA@</x:t>
+  </x:si>
+  <x:si>
+    <x:t>HoaiBao</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -1043,6 +1046,14 @@
         <x:v>3</x:v>
       </x:c>
     </x:row>
+    <x:row r="3" spans="1:2">
+      <x:c r="A3" s="0" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="B3" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>

</xml_diff>

<commit_message>
cap nhat giao dien
</commit_message>
<xml_diff>
--- a/QuanLyChiTieu/Data/Account.xlsx
+++ b/QuanLyChiTieu/Data/Account.xlsx
@@ -40,6 +40,9 @@
   </x:si>
   <x:si>
     <x:t>123456aA@</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Phuc123123</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -1043,6 +1046,14 @@
         <x:v>3</x:v>
       </x:c>
     </x:row>
+    <x:row r="3" spans="1:2">
+      <x:c r="A3" s="0" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="B3" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>

</xml_diff>

<commit_message>
sua loi du lieu
</commit_message>
<xml_diff>
--- a/QuanLyChiTieu/Data/Account.xlsx
+++ b/QuanLyChiTieu/Data/Account.xlsx
@@ -36,13 +36,19 @@
     <x:t>Mật khẩu</x:t>
   </x:si>
   <x:si>
-    <x:t>nha123vo</x:t>
+    <x:t>kikaho</x:t>
   </x:si>
   <x:si>
     <x:t>123456aA@</x:t>
   </x:si>
   <x:si>
-    <x:t>Phuc123123</x:t>
+    <x:t>abc</x:t>
+  </x:si>
+  <x:si>
+    <x:t>123</x:t>
+  </x:si>
+  <x:si>
+    <x:t>zcx</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -724,8 +730,8 @@
     <x:cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </x:cellStyles>
   <x:tableStyles count="2" defaultTableStyle="TableStylePreset3_Accent1 1" defaultPivotStyle="PivotStylePreset2_Accent1 1">
-    <x:tableStyle name="TableStylePreset3_Accent1 1" pivot="0" count="0" xr9:uid="{25B79EC9-D816-486E-A97A-BF66E5326128}"/>
-    <x:tableStyle name="PivotStylePreset2_Accent1 1" table="0" count="0" xr9:uid="{1985F190-A27A-48B5-A848-F692489BD1BD}"/>
+    <x:tableStyle name="TableStylePreset3_Accent1 1" pivot="0" count="0" xr9:uid="{6194AB5D-F443-46BF-8E34-5268C9AFA863}"/>
+    <x:tableStyle name="PivotStylePreset2_Accent1 1" table="0" count="0" xr9:uid="{940B6CFE-91C5-4CC3-BE3E-F3B748D91D05}"/>
   </x:tableStyles>
   <x:extLst>
     <x:ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1022,15 +1028,15 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:B1"/>
+  <x:dimension ref="A1:E2"/>
   <x:sheetViews>
     <x:sheetView tabSelected="1" workbookViewId="0">
-      <x:selection activeCell="A2" sqref="A2 A2:B5"/>
+      <x:selection activeCell="A2" sqref="A2 A2:B2"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultColWidth="8.996339" defaultRowHeight="14.4"/>
   <x:sheetData>
-    <x:row r="1" spans="1:2">
+    <x:row r="1" spans="1:5">
       <x:c r="A1" s="0" t="s">
         <x:v>0</x:v>
       </x:c>
@@ -1038,20 +1044,21 @@
         <x:v>1</x:v>
       </x:c>
     </x:row>
-    <x:row r="2" spans="1:2">
+    <x:row r="2" spans="1:5">
       <x:c r="A2" s="0" t="s">
         <x:v>2</x:v>
       </x:c>
       <x:c r="B2" s="0" t="s">
         <x:v>3</x:v>
       </x:c>
-    </x:row>
-    <x:row r="3" spans="1:2">
-      <x:c r="A3" s="0" t="s">
+      <x:c r="C2" s="0" t="s">
         <x:v>4</x:v>
       </x:c>
-      <x:c r="B3" s="0" t="s">
-        <x:v>3</x:v>
+      <x:c r="D2" s="0" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="E2" s="0" t="s">
+        <x:v>6</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
chỉnh phần báo cáo
</commit_message>
<xml_diff>
--- a/QuanLyChiTieu/Data/Account.xlsx
+++ b/QuanLyChiTieu/Data/Account.xlsx
@@ -43,6 +43,9 @@
   </x:si>
   <x:si>
     <x:t>Phuc123123</x:t>
+  </x:si>
+  <x:si>
+    <x:t>HoaiBao</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -1054,6 +1057,14 @@
         <x:v>3</x:v>
       </x:c>
     </x:row>
+    <x:row r="4" spans="1:2">
+      <x:c r="A4" s="0" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="B4" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>

</xml_diff>

<commit_message>
xu ly loi do push
</commit_message>
<xml_diff>
--- a/QuanLyChiTieu/Data/Account.xlsx
+++ b/QuanLyChiTieu/Data/Account.xlsx
@@ -39,16 +39,10 @@
     <x:t>kikaho</x:t>
   </x:si>
   <x:si>
-    <x:t>123456aA@</x:t>
+    <x:t/>
   </x:si>
   <x:si>
-    <x:t>abc</x:t>
-  </x:si>
-  <x:si>
-    <x:t>123</x:t>
-  </x:si>
-  <x:si>
-    <x:t>zcx</x:t>
+    <x:t>Nhacc123@</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -730,8 +724,8 @@
     <x:cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </x:cellStyles>
   <x:tableStyles count="2" defaultTableStyle="TableStylePreset3_Accent1 1" defaultPivotStyle="PivotStylePreset2_Accent1 1">
-    <x:tableStyle name="TableStylePreset3_Accent1 1" pivot="0" count="0" xr9:uid="{6194AB5D-F443-46BF-8E34-5268C9AFA863}"/>
-    <x:tableStyle name="PivotStylePreset2_Accent1 1" table="0" count="0" xr9:uid="{940B6CFE-91C5-4CC3-BE3E-F3B748D91D05}"/>
+    <x:tableStyle name="TableStylePreset3_Accent1 1" pivot="0" count="0" xr9:uid="{6E196651-3209-4B56-A559-BF6625764AD7}"/>
+    <x:tableStyle name="PivotStylePreset2_Accent1 1" table="0" count="0" xr9:uid="{5C10B57B-E938-4853-A5B6-F7304E3777CF}"/>
   </x:tableStyles>
   <x:extLst>
     <x:ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1028,10 +1022,10 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:E2"/>
+  <x:dimension ref="A1:B1"/>
   <x:sheetViews>
     <x:sheetView tabSelected="1" workbookViewId="0">
-      <x:selection activeCell="A2" sqref="A2 A2:B2"/>
+      <x:selection activeCell="A2" sqref="A2 A2:E2"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultColWidth="8.996339" defaultRowHeight="14.4"/>
@@ -1049,16 +1043,16 @@
         <x:v>2</x:v>
       </x:c>
       <x:c r="B2" s="0" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="C2" s="0" t="s">
         <x:v>3</x:v>
       </x:c>
-      <x:c r="C2" s="0" t="s">
-        <x:v>4</x:v>
-      </x:c>
       <x:c r="D2" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="E2" s="0" t="s">
-        <x:v>6</x:v>
+        <x:v>3</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
thanh toan khoan vay
</commit_message>
<xml_diff>
--- a/QuanLyChiTieu/Data/Account.xlsx
+++ b/QuanLyChiTieu/Data/Account.xlsx
@@ -1,38 +1,218 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<x:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<x:workbook xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <x:fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <x:workbookPr codeName="ThisWorkbook"/>
   <x:bookViews>
-    <x:workbookView firstSheet="0" activeTab="0"/>
+    <x:workbookView windowWidth="23040" windowHeight="9000" firstSheet="0" activeTab="0"/>
   </x:bookViews>
   <x:sheets>
-    <x:sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <x:sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </x:sheets>
   <x:definedNames/>
-  <x:calcPr calcId="125725"/>
+  <x:calcPr calcId="191029"/>
+  <x:extLst>
+    <x:ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </x:ext>
+  </x:extLst>
 </x:workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:si>
-    <x:t>123456aA@</x:t>
+    <x:t>a</x:t>
+  </x:si>
+  <x:si>
+    <x:t>b</x:t>
   </x:si>
   <x:si>
     <x:t/>
   </x:si>
   <x:si>
-    <x:t>HoaiBao</x:t>
+    <x:t>kikaho</x:t>
+  </x:si>
+  <x:si>
+    <x:t>123456aA@</x:t>
   </x:si>
 </x:sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<x:styleSheet xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <x:numFmts count="1">
-    <x:numFmt numFmtId="0" formatCode=""/>
+<x:styleSheet xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="xr9">
+  <x:numFmts count="4">
+    <x:numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <x:numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <x:numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <x:numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </x:numFmts>
-  <x:fonts count="1">
+  <x:fonts count="22">
+    <x:font>
+      <x:sz val="11"/>
+      <x:color rgb="FF000000"/>
+      <x:name val="Calibri"/>
+      <x:charset val="134"/>
+    </x:font>
+    <x:font>
+      <x:sz val="11"/>
+      <x:color theme="1"/>
+      <x:name val="Calibri"/>
+      <x:charset val="134"/>
+      <x:scheme val="minor"/>
+    </x:font>
+    <x:font>
+      <x:u/>
+      <x:sz val="11"/>
+      <x:color rgb="FF0000FF"/>
+      <x:name val="Calibri"/>
+      <x:charset val="0"/>
+      <x:scheme val="minor"/>
+    </x:font>
+    <x:font>
+      <x:u/>
+      <x:sz val="11"/>
+      <x:color rgb="FF800080"/>
+      <x:name val="Calibri"/>
+      <x:charset val="0"/>
+      <x:scheme val="minor"/>
+    </x:font>
+    <x:font>
+      <x:sz val="11"/>
+      <x:color rgb="FFFF0000"/>
+      <x:name val="Calibri"/>
+      <x:charset val="0"/>
+      <x:scheme val="minor"/>
+    </x:font>
+    <x:font>
+      <x:b/>
+      <x:sz val="18"/>
+      <x:color theme="3"/>
+      <x:name val="Calibri"/>
+      <x:charset val="134"/>
+      <x:scheme val="minor"/>
+    </x:font>
+    <x:font>
+      <x:i/>
+      <x:sz val="11"/>
+      <x:color rgb="FF7F7F7F"/>
+      <x:name val="Calibri"/>
+      <x:charset val="0"/>
+      <x:scheme val="minor"/>
+    </x:font>
+    <x:font>
+      <x:b/>
+      <x:sz val="15"/>
+      <x:color theme="3"/>
+      <x:name val="Calibri"/>
+      <x:charset val="134"/>
+      <x:scheme val="minor"/>
+    </x:font>
+    <x:font>
+      <x:b/>
+      <x:sz val="13"/>
+      <x:color theme="3"/>
+      <x:name val="Calibri"/>
+      <x:charset val="134"/>
+      <x:scheme val="minor"/>
+    </x:font>
+    <x:font>
+      <x:b/>
+      <x:sz val="11"/>
+      <x:color theme="3"/>
+      <x:name val="Calibri"/>
+      <x:charset val="134"/>
+      <x:scheme val="minor"/>
+    </x:font>
+    <x:font>
+      <x:sz val="11"/>
+      <x:color rgb="FF3F3F76"/>
+      <x:name val="Calibri"/>
+      <x:charset val="0"/>
+      <x:scheme val="minor"/>
+    </x:font>
+    <x:font>
+      <x:b/>
+      <x:sz val="11"/>
+      <x:color rgb="FF3F3F3F"/>
+      <x:name val="Calibri"/>
+      <x:charset val="0"/>
+      <x:scheme val="minor"/>
+    </x:font>
+    <x:font>
+      <x:b/>
+      <x:sz val="11"/>
+      <x:color rgb="FFFA7D00"/>
+      <x:name val="Calibri"/>
+      <x:charset val="0"/>
+      <x:scheme val="minor"/>
+    </x:font>
+    <x:font>
+      <x:b/>
+      <x:sz val="11"/>
+      <x:color rgb="FFFFFFFF"/>
+      <x:name val="Calibri"/>
+      <x:charset val="0"/>
+      <x:scheme val="minor"/>
+    </x:font>
+    <x:font>
+      <x:sz val="11"/>
+      <x:color rgb="FFFA7D00"/>
+      <x:name val="Calibri"/>
+      <x:charset val="0"/>
+      <x:scheme val="minor"/>
+    </x:font>
+    <x:font>
+      <x:b/>
+      <x:sz val="11"/>
+      <x:color theme="1"/>
+      <x:name val="Calibri"/>
+      <x:charset val="0"/>
+      <x:scheme val="minor"/>
+    </x:font>
+    <x:font>
+      <x:sz val="11"/>
+      <x:color rgb="FF006100"/>
+      <x:name val="Calibri"/>
+      <x:charset val="0"/>
+      <x:scheme val="minor"/>
+    </x:font>
+    <x:font>
+      <x:sz val="11"/>
+      <x:color rgb="FF9C0006"/>
+      <x:name val="Calibri"/>
+      <x:charset val="0"/>
+      <x:scheme val="minor"/>
+    </x:font>
+    <x:font>
+      <x:sz val="11"/>
+      <x:color rgb="FF9C6500"/>
+      <x:name val="Calibri"/>
+      <x:charset val="0"/>
+      <x:scheme val="minor"/>
+    </x:font>
+    <x:font>
+      <x:sz val="11"/>
+      <x:color theme="0"/>
+      <x:name val="Calibri"/>
+      <x:charset val="0"/>
+      <x:scheme val="minor"/>
+    </x:font>
+    <x:font>
+      <x:sz val="11"/>
+      <x:color theme="1"/>
+      <x:name val="Calibri"/>
+      <x:charset val="0"/>
+      <x:scheme val="minor"/>
+    </x:font>
     <x:font>
       <x:vertAlign val="baseline"/>
       <x:sz val="11"/>
@@ -41,47 +221,517 @@
       <x:family val="2"/>
     </x:font>
   </x:fonts>
-  <x:fills count="2">
+  <x:fills count="33">
     <x:fill>
       <x:patternFill patternType="none"/>
     </x:fill>
     <x:fill>
       <x:patternFill patternType="gray125"/>
     </x:fill>
+    <x:fill>
+      <x:patternFill patternType="solid">
+        <x:fgColor rgb="FFFFFFCC"/>
+        <x:bgColor indexed="64"/>
+      </x:patternFill>
+    </x:fill>
+    <x:fill>
+      <x:patternFill patternType="solid">
+        <x:fgColor rgb="FFFFCC99"/>
+        <x:bgColor indexed="64"/>
+      </x:patternFill>
+    </x:fill>
+    <x:fill>
+      <x:patternFill patternType="solid">
+        <x:fgColor rgb="FFF2F2F2"/>
+        <x:bgColor indexed="64"/>
+      </x:patternFill>
+    </x:fill>
+    <x:fill>
+      <x:patternFill patternType="solid">
+        <x:fgColor rgb="FFA5A5A5"/>
+        <x:bgColor indexed="64"/>
+      </x:patternFill>
+    </x:fill>
+    <x:fill>
+      <x:patternFill patternType="solid">
+        <x:fgColor rgb="FFC6EFCE"/>
+        <x:bgColor indexed="64"/>
+      </x:patternFill>
+    </x:fill>
+    <x:fill>
+      <x:patternFill patternType="solid">
+        <x:fgColor rgb="FFFFC7CE"/>
+        <x:bgColor indexed="64"/>
+      </x:patternFill>
+    </x:fill>
+    <x:fill>
+      <x:patternFill patternType="solid">
+        <x:fgColor rgb="FFFFEB9C"/>
+        <x:bgColor indexed="64"/>
+      </x:patternFill>
+    </x:fill>
+    <x:fill>
+      <x:patternFill patternType="solid">
+        <x:fgColor theme="4"/>
+        <x:bgColor indexed="64"/>
+      </x:patternFill>
+    </x:fill>
+    <x:fill>
+      <x:patternFill patternType="solid">
+        <x:fgColor theme="4" tint="0.799981688894314"/>
+        <x:bgColor indexed="64"/>
+      </x:patternFill>
+    </x:fill>
+    <x:fill>
+      <x:patternFill patternType="solid">
+        <x:fgColor theme="4" tint="0.599993896298105"/>
+        <x:bgColor indexed="64"/>
+      </x:patternFill>
+    </x:fill>
+    <x:fill>
+      <x:patternFill patternType="solid">
+        <x:fgColor theme="4" tint="0.399975585192419"/>
+        <x:bgColor indexed="64"/>
+      </x:patternFill>
+    </x:fill>
+    <x:fill>
+      <x:patternFill patternType="solid">
+        <x:fgColor theme="5"/>
+        <x:bgColor indexed="64"/>
+      </x:patternFill>
+    </x:fill>
+    <x:fill>
+      <x:patternFill patternType="solid">
+        <x:fgColor theme="5" tint="0.799981688894314"/>
+        <x:bgColor indexed="64"/>
+      </x:patternFill>
+    </x:fill>
+    <x:fill>
+      <x:patternFill patternType="solid">
+        <x:fgColor theme="5" tint="0.599993896298105"/>
+        <x:bgColor indexed="64"/>
+      </x:patternFill>
+    </x:fill>
+    <x:fill>
+      <x:patternFill patternType="solid">
+        <x:fgColor theme="5" tint="0.399975585192419"/>
+        <x:bgColor indexed="64"/>
+      </x:patternFill>
+    </x:fill>
+    <x:fill>
+      <x:patternFill patternType="solid">
+        <x:fgColor theme="6"/>
+        <x:bgColor indexed="64"/>
+      </x:patternFill>
+    </x:fill>
+    <x:fill>
+      <x:patternFill patternType="solid">
+        <x:fgColor theme="6" tint="0.799981688894314"/>
+        <x:bgColor indexed="64"/>
+      </x:patternFill>
+    </x:fill>
+    <x:fill>
+      <x:patternFill patternType="solid">
+        <x:fgColor theme="6" tint="0.599993896298105"/>
+        <x:bgColor indexed="64"/>
+      </x:patternFill>
+    </x:fill>
+    <x:fill>
+      <x:patternFill patternType="solid">
+        <x:fgColor theme="6" tint="0.399975585192419"/>
+        <x:bgColor indexed="64"/>
+      </x:patternFill>
+    </x:fill>
+    <x:fill>
+      <x:patternFill patternType="solid">
+        <x:fgColor theme="7"/>
+        <x:bgColor indexed="64"/>
+      </x:patternFill>
+    </x:fill>
+    <x:fill>
+      <x:patternFill patternType="solid">
+        <x:fgColor theme="7" tint="0.799981688894314"/>
+        <x:bgColor indexed="64"/>
+      </x:patternFill>
+    </x:fill>
+    <x:fill>
+      <x:patternFill patternType="solid">
+        <x:fgColor theme="7" tint="0.599993896298105"/>
+        <x:bgColor indexed="64"/>
+      </x:patternFill>
+    </x:fill>
+    <x:fill>
+      <x:patternFill patternType="solid">
+        <x:fgColor theme="7" tint="0.399975585192419"/>
+        <x:bgColor indexed="64"/>
+      </x:patternFill>
+    </x:fill>
+    <x:fill>
+      <x:patternFill patternType="solid">
+        <x:fgColor theme="8"/>
+        <x:bgColor indexed="64"/>
+      </x:patternFill>
+    </x:fill>
+    <x:fill>
+      <x:patternFill patternType="solid">
+        <x:fgColor theme="8" tint="0.799981688894314"/>
+        <x:bgColor indexed="64"/>
+      </x:patternFill>
+    </x:fill>
+    <x:fill>
+      <x:patternFill patternType="solid">
+        <x:fgColor theme="8" tint="0.599993896298105"/>
+        <x:bgColor indexed="64"/>
+      </x:patternFill>
+    </x:fill>
+    <x:fill>
+      <x:patternFill patternType="solid">
+        <x:fgColor theme="8" tint="0.399975585192419"/>
+        <x:bgColor indexed="64"/>
+      </x:patternFill>
+    </x:fill>
+    <x:fill>
+      <x:patternFill patternType="solid">
+        <x:fgColor theme="9"/>
+        <x:bgColor indexed="64"/>
+      </x:patternFill>
+    </x:fill>
+    <x:fill>
+      <x:patternFill patternType="solid">
+        <x:fgColor theme="9" tint="0.799981688894314"/>
+        <x:bgColor indexed="64"/>
+      </x:patternFill>
+    </x:fill>
+    <x:fill>
+      <x:patternFill patternType="solid">
+        <x:fgColor theme="9" tint="0.599993896298105"/>
+        <x:bgColor indexed="64"/>
+      </x:patternFill>
+    </x:fill>
+    <x:fill>
+      <x:patternFill patternType="solid">
+        <x:fgColor theme="9" tint="0.399975585192419"/>
+        <x:bgColor indexed="64"/>
+      </x:patternFill>
+    </x:fill>
   </x:fills>
-  <x:borders count="1">
-    <x:border diagonalUp="0" diagonalDown="0">
-      <x:left style="none">
-        <x:color rgb="FF000000"/>
+  <x:borders count="9">
+    <x:border>
+      <x:left/>
+      <x:right/>
+      <x:top/>
+      <x:bottom/>
+      <x:diagonal/>
+    </x:border>
+    <x:border>
+      <x:left style="thin">
+        <x:color rgb="FFB2B2B2"/>
       </x:left>
-      <x:right style="none">
-        <x:color rgb="FF000000"/>
+      <x:right style="thin">
+        <x:color rgb="FFB2B2B2"/>
       </x:right>
-      <x:top style="none">
-        <x:color rgb="FF000000"/>
+      <x:top style="thin">
+        <x:color rgb="FFB2B2B2"/>
       </x:top>
-      <x:bottom style="none">
-        <x:color rgb="FF000000"/>
+      <x:bottom style="thin">
+        <x:color rgb="FFB2B2B2"/>
       </x:bottom>
-      <x:diagonal style="none">
-        <x:color rgb="FF000000"/>
-      </x:diagonal>
+      <x:diagonal/>
+    </x:border>
+    <x:border>
+      <x:left/>
+      <x:right/>
+      <x:top/>
+      <x:bottom style="medium">
+        <x:color theme="4"/>
+      </x:bottom>
+      <x:diagonal/>
+    </x:border>
+    <x:border>
+      <x:left/>
+      <x:right/>
+      <x:top/>
+      <x:bottom style="medium">
+        <x:color theme="4" tint="0.499984740745262"/>
+      </x:bottom>
+      <x:diagonal/>
+    </x:border>
+    <x:border>
+      <x:left style="thin">
+        <x:color rgb="FF7F7F7F"/>
+      </x:left>
+      <x:right style="thin">
+        <x:color rgb="FF7F7F7F"/>
+      </x:right>
+      <x:top style="thin">
+        <x:color rgb="FF7F7F7F"/>
+      </x:top>
+      <x:bottom style="thin">
+        <x:color rgb="FF7F7F7F"/>
+      </x:bottom>
+      <x:diagonal/>
+    </x:border>
+    <x:border>
+      <x:left style="thin">
+        <x:color rgb="FF3F3F3F"/>
+      </x:left>
+      <x:right style="thin">
+        <x:color rgb="FF3F3F3F"/>
+      </x:right>
+      <x:top style="thin">
+        <x:color rgb="FF3F3F3F"/>
+      </x:top>
+      <x:bottom style="thin">
+        <x:color rgb="FF3F3F3F"/>
+      </x:bottom>
+      <x:diagonal/>
+    </x:border>
+    <x:border>
+      <x:left style="double">
+        <x:color rgb="FF3F3F3F"/>
+      </x:left>
+      <x:right style="double">
+        <x:color rgb="FF3F3F3F"/>
+      </x:right>
+      <x:top style="double">
+        <x:color rgb="FF3F3F3F"/>
+      </x:top>
+      <x:bottom style="double">
+        <x:color rgb="FF3F3F3F"/>
+      </x:bottom>
+      <x:diagonal/>
+    </x:border>
+    <x:border>
+      <x:left/>
+      <x:right/>
+      <x:top/>
+      <x:bottom style="double">
+        <x:color rgb="FFFF8001"/>
+      </x:bottom>
+      <x:diagonal/>
+    </x:border>
+    <x:border>
+      <x:left/>
+      <x:right/>
+      <x:top style="thin">
+        <x:color theme="4"/>
+      </x:top>
+      <x:bottom style="double">
+        <x:color theme="4"/>
+      </x:bottom>
+      <x:diagonal/>
     </x:border>
   </x:borders>
-  <x:cellStyleXfs count="1">
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
+  <x:cellStyleXfs count="49">
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="0"/>
+    <x:xf numFmtId="176" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <x:alignment vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <x:alignment vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <x:alignment vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="177" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <x:alignment vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <x:alignment vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <x:alignment vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <x:alignment vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <x:alignment vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <x:alignment vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <x:alignment vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <x:alignment vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <x:alignment vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <x:alignment vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <x:alignment vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <x:alignment vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="10" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <x:alignment vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <x:alignment vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="12" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <x:alignment vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="13" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <x:alignment vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <x:alignment vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <x:alignment vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <x:alignment vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <x:alignment vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <x:alignment vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <x:alignment vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <x:alignment vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <x:alignment vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <x:alignment vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <x:alignment vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <x:alignment vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <x:alignment vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <x:alignment vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <x:alignment vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <x:alignment vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <x:alignment vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <x:alignment vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <x:alignment vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <x:alignment vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <x:alignment vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <x:alignment vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <x:alignment vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <x:alignment vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <x:alignment vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <x:alignment vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <x:alignment vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <x:alignment vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <x:alignment vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <x:alignment vertical="center"/>
     </x:xf>
   </x:cellStyleXfs>
   <x:cellXfs count="1">
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
   </x:cellXfs>
-  <x:cellStyles count="1">
+  <x:cellStyles count="49">
     <x:cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <x:cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <x:cellStyle name="Currency" xfId="2" builtinId="4"/>
+    <x:cellStyle name="Percent" xfId="3" builtinId="5"/>
+    <x:cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
+    <x:cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
+    <x:cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
+    <x:cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
+    <x:cellStyle name="Note" xfId="8" builtinId="10"/>
+    <x:cellStyle name="Warning Text" xfId="9" builtinId="11"/>
+    <x:cellStyle name="Title" xfId="10" builtinId="15"/>
+    <x:cellStyle name="CExplanatory Text" xfId="11" builtinId="53"/>
+    <x:cellStyle name="Heading 1" xfId="12" builtinId="16"/>
+    <x:cellStyle name="Heading 2" xfId="13" builtinId="17"/>
+    <x:cellStyle name="Heading 3" xfId="14" builtinId="18"/>
+    <x:cellStyle name="Heading 4" xfId="15" builtinId="19"/>
+    <x:cellStyle name="Input" xfId="16" builtinId="20"/>
+    <x:cellStyle name="Output" xfId="17" builtinId="21"/>
+    <x:cellStyle name="Calculation" xfId="18" builtinId="22"/>
+    <x:cellStyle name="Check Cell" xfId="19" builtinId="23"/>
+    <x:cellStyle name="Linked Cell" xfId="20" builtinId="24"/>
+    <x:cellStyle name="Total" xfId="21" builtinId="25"/>
+    <x:cellStyle name="Good" xfId="22" builtinId="26"/>
+    <x:cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <x:cellStyle name="Neutral" xfId="24" builtinId="28"/>
+    <x:cellStyle name="Accent1" xfId="25" builtinId="29"/>
+    <x:cellStyle name="20% - Accent1" xfId="26" builtinId="30"/>
+    <x:cellStyle name="40% - Accent1" xfId="27" builtinId="31"/>
+    <x:cellStyle name="60% - Accent1" xfId="28" builtinId="32"/>
+    <x:cellStyle name="Accent2" xfId="29" builtinId="33"/>
+    <x:cellStyle name="20% - Accent2" xfId="30" builtinId="34"/>
+    <x:cellStyle name="40% - Accent2" xfId="31" builtinId="35"/>
+    <x:cellStyle name="60% - Accent2" xfId="32" builtinId="36"/>
+    <x:cellStyle name="Accent3" xfId="33" builtinId="37"/>
+    <x:cellStyle name="20% - Accent3" xfId="34" builtinId="38"/>
+    <x:cellStyle name="40% - Accent3" xfId="35" builtinId="39"/>
+    <x:cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
+    <x:cellStyle name="Accent4" xfId="37" builtinId="41"/>
+    <x:cellStyle name="20% - Accent4" xfId="38" builtinId="42"/>
+    <x:cellStyle name="40% - Accent4" xfId="39" builtinId="43"/>
+    <x:cellStyle name="60% - Accent4" xfId="40" builtinId="44"/>
+    <x:cellStyle name="Accent5" xfId="41" builtinId="45"/>
+    <x:cellStyle name="20% - Accent5" xfId="42" builtinId="46"/>
+    <x:cellStyle name="40% - Accent5" xfId="43" builtinId="47"/>
+    <x:cellStyle name="60% - Accent5" xfId="44" builtinId="48"/>
+    <x:cellStyle name="Accent6" xfId="45" builtinId="49"/>
+    <x:cellStyle name="20% - Accent6" xfId="46" builtinId="50"/>
+    <x:cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <x:cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </x:cellStyles>
+  <x:tableStyles count="2" defaultTableStyle="TableStylePreset3_Accent1 1" defaultPivotStyle="PivotStylePreset2_Accent1 1">
+    <x:tableStyle name="TableStylePreset3_Accent1 1" pivot="0" count="0" xr9:uid="{F2E48A53-B6B8-4BA0-BA84-6B1EADFD9CC6}"/>
+    <x:tableStyle name="PivotStylePreset2_Accent1 1" table="0" count="0" xr9:uid="{C7D320BE-D80A-4289-81A2-68DAB2DA1343}"/>
+  </x:tableStyles>
+  <x:extLst>
+    <x:ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </x:ext>
+  </x:extLst>
 </x:styleSheet>
 </file>
 
@@ -364,42 +1014,51 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac">
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac">
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
   <x:dimension ref="A1:E2"/>
   <x:sheetViews>
-    <x:sheetView workbookViewId="0"/>
+    <x:sheetView tabSelected="1" workbookViewId="0">
+      <x:selection activeCell="A2" sqref="A2 A2:B2"/>
+    </x:sheetView>
   </x:sheetViews>
-  <x:sheetFormatPr defaultRowHeight="15"/>
+  <x:sheetFormatPr defaultColWidth="8.996339" defaultRowHeight="14.4"/>
   <x:sheetData>
+    <x:row r="1" spans="1:5">
+      <x:c r="A1" s="0" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="B1" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+    </x:row>
     <x:row r="2" spans="1:5">
       <x:c r="A2" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="B2" s="0" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="C2" s="0" t="s">
         <x:v>2</x:v>
       </x:c>
-      <x:c r="B2" s="0" t="s">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="C2" s="0" t="s">
-        <x:v>1</x:v>
-      </x:c>
       <x:c r="D2" s="0" t="s">
-        <x:v>1</x:v>
+        <x:v>2</x:v>
       </x:c>
       <x:c r="E2" s="0" t="s">
-        <x:v>1</x:v>
+        <x:v>2</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
-  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
+  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="portrait" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
   <x:headerFooter/>
   <x:tableParts count="0"/>
 </x:worksheet>

</xml_diff>